<commit_message>
Updated ACE landing page with HLSR 2021 data
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A0155F61-7DD8-403F-90C7-ECD565C036E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B622B777-9B7E-42DD-B348-FFD332B4E535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACE_landing_page_data" sheetId="1" r:id="rId1"/>
     <sheet name="ANSP" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -188,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1064,10 +1077,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1120,278 +1135,278 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2">
-        <v>866.11622269999998</v>
+        <v>662.75700797706486</v>
       </c>
       <c r="C2">
-        <v>8210637056</v>
+        <v>7941263394.7824574</v>
       </c>
       <c r="D2">
-        <v>9479832.8920000009</v>
+        <v>11982164.351640126</v>
       </c>
       <c r="E2">
-        <v>0.47213889399999998</v>
+        <v>0.60158469058868869</v>
       </c>
       <c r="F2">
-        <v>130.63126159999999</v>
+        <v>125.39389272546444</v>
       </c>
       <c r="G2">
-        <v>589.43649289999996</v>
+        <v>454.31770643373841</v>
       </c>
       <c r="H2">
-        <v>1.199004827</v>
+        <v>-0.25254822055608572</v>
       </c>
       <c r="I2">
-        <v>-5.2007629E-2</v>
+        <v>-4.8469911156530432E-2</v>
       </c>
       <c r="J2">
-        <v>-0.56889936799999996</v>
+        <v>0.27303207378994321</v>
       </c>
       <c r="K2">
-        <v>-0.49692409799999998</v>
+        <v>0.25316859156402782</v>
       </c>
       <c r="L2">
-        <v>0.105249041</v>
+        <v>-8.3792408393972728E-2</v>
       </c>
       <c r="M2">
-        <v>1.1999553030000001</v>
+        <v>-0.24480503428890987</v>
       </c>
       <c r="N2">
-        <v>99.812170089999995</v>
+        <v>94.781119663628346</v>
       </c>
       <c r="O2">
-        <v>49.663693729999999</v>
+        <v>61.747354520507066</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B3">
-        <v>393.86735850000002</v>
+        <v>886.68864828998028</v>
       </c>
       <c r="C3">
-        <v>8661079249</v>
+        <v>8345782742.8606167</v>
       </c>
       <c r="D3">
-        <v>21989837.600000001</v>
+        <v>9412303.5847541764</v>
       </c>
       <c r="E3">
-        <v>0.93850429400000002</v>
+        <v>0.48005088432504983</v>
       </c>
       <c r="F3">
-        <v>118.1916987</v>
+        <v>136.86187920104496</v>
       </c>
       <c r="G3">
-        <v>267.93112200000002</v>
+        <v>601.58995631803998</v>
       </c>
       <c r="H3">
-        <v>5.4513100000000002E-4</v>
+        <v>1.2155110234593454</v>
       </c>
       <c r="I3">
-        <v>1.7838621999999998E-2</v>
+        <v>-4.1009837022952467E-2</v>
       </c>
       <c r="J3">
-        <v>1.7284068999999999E-2</v>
+        <v>-0.56714719411341041</v>
       </c>
       <c r="K3">
-        <v>1.0509449000000001E-2</v>
+        <v>-0.50717079833904599</v>
       </c>
       <c r="L3">
-        <v>8.8013150000000005E-3</v>
+        <v>8.6295156755763491E-2</v>
       </c>
       <c r="M3">
-        <v>1.59935E-3</v>
+        <v>1.2209110515285637</v>
       </c>
       <c r="N3">
-        <v>105.2879465</v>
+        <v>99.609167145549108</v>
       </c>
       <c r="O3">
-        <v>115.2020898</v>
+        <v>48.50416245733625</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B4">
-        <v>393.6527663</v>
+        <v>400.21856759055345</v>
       </c>
       <c r="C4">
-        <v>8509285328</v>
+        <v>8702678155.6886158</v>
       </c>
       <c r="D4">
-        <v>21616221.34</v>
+        <v>21744813.610426877</v>
       </c>
       <c r="E4">
-        <v>0.92874370900000003</v>
+        <v>0.97407150937314968</v>
       </c>
       <c r="F4">
-        <v>117.1605319</v>
+        <v>125.9895879585664</v>
       </c>
       <c r="G4">
-        <v>267.50329060000001</v>
+        <v>270.8753040352471</v>
       </c>
       <c r="H4">
-        <v>-3.3033864000000003E-2</v>
+        <v>-2.4749120278552139E-3</v>
       </c>
       <c r="I4">
-        <v>1.9480196000000002E-2</v>
+        <v>1.4080730999245228E-2</v>
       </c>
       <c r="J4">
-        <v>5.4308065000000003E-2</v>
+        <v>1.6596718445203384E-2</v>
       </c>
       <c r="K4">
-        <v>5.3407649000000001E-2</v>
+        <v>1.0175199012249392E-2</v>
       </c>
       <c r="L4">
-        <v>4.7576559999999999E-3</v>
+        <v>6.3459591994667885E-3</v>
       </c>
       <c r="M4">
-        <v>-2.6706143000000002E-2</v>
+        <v>-1.8454097782281131E-3</v>
       </c>
       <c r="N4">
-        <v>103.4426718</v>
+        <v>103.86881012035278</v>
       </c>
       <c r="O4">
-        <v>113.24475959999999</v>
+        <v>112.0569436023124</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B5">
-        <v>407.10088150000001</v>
+        <v>401.21153083392852</v>
       </c>
       <c r="C5">
-        <v>8346690168</v>
+        <v>8581839581.0689087</v>
       </c>
       <c r="D5">
-        <v>20502756.309999999</v>
+        <v>21389812.907997269</v>
       </c>
       <c r="E5">
-        <v>0.88165650799999995</v>
+        <v>0.96425997225589977</v>
       </c>
       <c r="F5">
-        <v>116.6057619</v>
+        <v>125.19510493070321</v>
       </c>
       <c r="G5">
-        <v>274.84329500000001</v>
+        <v>271.37610415142558</v>
       </c>
       <c r="H5">
-        <v>-3.6078579E-2</v>
+        <v>-3.6100637895362109E-2</v>
       </c>
       <c r="I5">
-        <v>1.0097406999999999E-2</v>
+        <v>1.5247568031038217E-2</v>
       </c>
       <c r="J5">
-        <v>4.7904304000000002E-2</v>
+        <v>5.3271335105236961E-2</v>
       </c>
       <c r="K5">
-        <v>4.1747010000000001E-2</v>
+        <v>4.9175437958467239E-2</v>
       </c>
       <c r="L5">
-        <v>1.0534623999999999E-2</v>
+        <v>-4.4919207430038632E-4</v>
       </c>
       <c r="M5">
-        <v>-3.8994734000000003E-2</v>
+        <v>-3.0649484459494225E-2</v>
       </c>
       <c r="N5">
-        <v>101.4660925</v>
+        <v>102.4265691529347</v>
       </c>
       <c r="O5">
-        <v>107.4114514</v>
+        <v>110.22752834938696</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B6">
-        <v>422.33824509999999</v>
+        <v>416.2379877064119</v>
       </c>
       <c r="C6">
-        <v>8263252745</v>
+        <v>8452952611.0684996</v>
       </c>
       <c r="D6">
-        <v>19565485.350000001</v>
+        <v>20307979.715274524</v>
       </c>
       <c r="E6">
-        <v>0.84632497100000004</v>
+        <v>0.91906456953681659</v>
       </c>
       <c r="F6">
-        <v>115.3901699</v>
+        <v>125.25136685198841</v>
       </c>
       <c r="G6">
-        <v>285.9956181</v>
+        <v>279.95663054876223</v>
       </c>
       <c r="H6">
-        <v>-1.9994036E-2</v>
+        <v>-3.5969301290042055E-2</v>
       </c>
       <c r="I6">
-        <v>4.5178989999999997E-3</v>
+        <v>8.8826841671716394E-3</v>
       </c>
       <c r="J6">
-        <v>2.5012026E-2</v>
+        <v>4.6525474258479083E-2</v>
       </c>
       <c r="K6">
-        <v>1.6368119E-2</v>
+        <v>4.2163773284719097E-2</v>
       </c>
       <c r="L6">
-        <v>1.5684433000000001E-2</v>
+        <v>1.1290411509540688E-2</v>
       </c>
       <c r="M6">
-        <v>-2.8944514000000001E-2</v>
+        <v>-3.9028085741710017E-2</v>
       </c>
       <c r="N6">
-        <v>100.45178989999999</v>
+        <v>100.88826841671717</v>
       </c>
       <c r="O6">
-        <v>102.5012026</v>
+        <v>104.65254742584791</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B7">
-        <v>430.95477019999998</v>
+        <v>431.76839520091141</v>
       </c>
       <c r="C7">
-        <v>8226088110</v>
+        <v>8378528786.0762281</v>
       </c>
       <c r="D7">
-        <v>19088054.43</v>
+        <v>19405146.090365212</v>
       </c>
       <c r="E7">
-        <v>0.83269531500000005</v>
+        <v>0.88188113336552165</v>
       </c>
       <c r="F7">
-        <v>113.6082883</v>
+        <v>123.85301534207888</v>
       </c>
       <c r="G7">
-        <v>294.52036709999999</v>
+        <v>291.32654804468666</v>
       </c>
       <c r="H7">
-        <v>-1.0284458E-2</v>
+        <v>-1.9204070002918572E-2</v>
       </c>
       <c r="I7">
-        <v>6.1185850000000002E-3</v>
+        <v>6.5683161127729761E-3</v>
       </c>
       <c r="J7">
-        <v>1.6573493000000002E-2</v>
+        <v>2.6277011687607876E-2</v>
       </c>
       <c r="K7">
-        <v>1.4085527E-2</v>
+        <v>1.8155459390721607E-2</v>
       </c>
       <c r="L7">
-        <v>1.6604437E-2</v>
+        <v>1.6252900049103847E-2</v>
       </c>
       <c r="M7">
-        <v>-1.6089729000000001E-2</v>
+        <v>-2.734775827991065E-2</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1406,10 +1421,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refreshed ace landing page data
</commit_message>
<xml_diff>
--- a/content/economics/ACE_landing_page_data.xlsx
+++ b/content/economics/ACE_landing_page_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oaolive\repos\portal\content\economics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BA86A8-12E1-4C9A-B475-53FEB71D63FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7B5B5-722D-456C-8F61-81668789581F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1138,46 +1138,46 @@
         <v>2021</v>
       </c>
       <c r="B2">
-        <v>662.75700797706486</v>
+        <v>662.85092446876183</v>
       </c>
       <c r="C2">
-        <v>7941263394.7824574</v>
+        <v>7937423242.1468859</v>
       </c>
       <c r="D2">
-        <v>11982164.351640126</v>
+        <v>11974673.262330122</v>
       </c>
       <c r="E2">
-        <v>0.60158469058868869</v>
+        <v>0.59923449274665208</v>
       </c>
       <c r="F2">
-        <v>125.39389272546444</v>
+        <v>125.21093692568316</v>
       </c>
       <c r="G2">
-        <v>454.31770643373841</v>
+        <v>453.89943979743367</v>
       </c>
       <c r="H2">
-        <v>-0.25254822055608572</v>
+        <v>-0.25232573453784612</v>
       </c>
       <c r="I2">
-        <v>-4.8469911156530432E-2</v>
+        <v>-4.8988431857763137E-2</v>
       </c>
       <c r="J2">
-        <v>0.27303207378994321</v>
+        <v>0.27195974513633403</v>
       </c>
       <c r="K2">
-        <v>0.25316859156402782</v>
+        <v>0.24800162609219956</v>
       </c>
       <c r="L2">
-        <v>-8.3792408393972728E-2</v>
+        <v>-8.4930924006279773E-2</v>
       </c>
       <c r="M2">
-        <v>-0.24480503428890987</v>
+        <v>-0.24548207898660512</v>
       </c>
       <c r="N2">
-        <v>94.781119663628346</v>
+        <v>94.735286406577842</v>
       </c>
       <c r="O2">
-        <v>61.747354520507066</v>
+        <v>61.694784529334171</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1185,46 +1185,46 @@
         <v>2020</v>
       </c>
       <c r="B3">
-        <v>886.68864828998028</v>
+        <v>886.55040716031488</v>
       </c>
       <c r="C3">
-        <v>8345782742.8606167</v>
+        <v>8346295153.5409031</v>
       </c>
       <c r="D3">
-        <v>9412303.5847541764</v>
+        <v>9414349.2418831438</v>
       </c>
       <c r="E3">
-        <v>0.48005088432504983</v>
+        <v>0.48015521792467764</v>
       </c>
       <c r="F3">
-        <v>136.86187920104496</v>
+        <v>136.83222415718748</v>
       </c>
       <c r="G3">
-        <v>601.58995631803998</v>
+        <v>601.57542605190906</v>
       </c>
       <c r="H3">
-        <v>1.2155110234593454</v>
+        <v>1.2156413238068402</v>
       </c>
       <c r="I3">
-        <v>-4.1009837022952467E-2</v>
+        <v>-4.0950957368767971E-2</v>
       </c>
       <c r="J3">
-        <v>-0.56714719411341041</v>
+        <v>-0.56714607534786987</v>
       </c>
       <c r="K3">
-        <v>-0.50717079833904599</v>
+        <v>-0.5071695245565484</v>
       </c>
       <c r="L3">
-        <v>8.6295156755763491E-2</v>
+        <v>8.605977981439894E-2</v>
       </c>
       <c r="M3">
-        <v>1.2209110515285637</v>
+        <v>1.2213343463924975</v>
       </c>
       <c r="N3">
-        <v>99.609167145549108</v>
+        <v>99.615282905169551</v>
       </c>
       <c r="O3">
-        <v>48.50416245733625</v>
+        <v>48.503724088156154</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1232,46 +1232,46 @@
         <v>2019</v>
       </c>
       <c r="B4">
-        <v>400.21856759055345</v>
+        <v>400.13263773085521</v>
       </c>
       <c r="C4">
         <v>8702678155.6886158</v>
       </c>
       <c r="D4">
-        <v>21744813.610426877</v>
+        <v>21749483.383913253</v>
       </c>
       <c r="E4">
-        <v>0.97407150937314968</v>
+        <v>0.97428069457886368</v>
       </c>
       <c r="F4">
-        <v>125.9895879585664</v>
+        <v>125.98958795856642</v>
       </c>
       <c r="G4">
-        <v>270.8753040352471</v>
+        <v>270.81714512220213</v>
       </c>
       <c r="H4">
-        <v>-2.4749120278552139E-3</v>
+        <v>-2.4712782600395666E-3</v>
       </c>
       <c r="I4">
-        <v>1.4080730999245228E-2</v>
+        <v>1.408073099924545E-2</v>
       </c>
       <c r="J4">
-        <v>1.6596718445203384E-2</v>
+        <v>1.659301521705947E-2</v>
       </c>
       <c r="K4">
-        <v>1.0175199012249392E-2</v>
+        <v>1.017151917622483E-2</v>
       </c>
       <c r="L4">
-        <v>6.3459591994667885E-3</v>
+        <v>6.3459591994670106E-3</v>
       </c>
       <c r="M4">
-        <v>-1.8454097782281131E-3</v>
+        <v>-1.8417737172722326E-3</v>
       </c>
       <c r="N4">
-        <v>103.86881012035278</v>
+        <v>103.86881012035276</v>
       </c>
       <c r="O4">
-        <v>112.0569436023124</v>
+        <v>112.05564123540506</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1279,46 +1279,46 @@
         <v>2018</v>
       </c>
       <c r="B5">
-        <v>401.21153083392852</v>
+        <v>401.12392657016977</v>
       </c>
       <c r="C5">
-        <v>8581839581.0689087</v>
+        <v>8581839581.0689077</v>
       </c>
       <c r="D5">
-        <v>21389812.907997269</v>
+        <v>21394484.379050527</v>
       </c>
       <c r="E5">
-        <v>0.96425997225589977</v>
+        <v>0.96447056374482887</v>
       </c>
       <c r="F5">
-        <v>125.19510493070321</v>
+        <v>125.19510493070318</v>
       </c>
       <c r="G5">
-        <v>271.37610415142558</v>
+        <v>271.31684936441462</v>
       </c>
       <c r="H5">
-        <v>-3.6100637895362109E-2</v>
+        <v>-3.6096055075297007E-2</v>
       </c>
       <c r="I5">
         <v>1.5247568031038217E-2</v>
       </c>
       <c r="J5">
-        <v>5.3271335105236961E-2</v>
+        <v>5.3266327393592938E-2</v>
       </c>
       <c r="K5">
-        <v>4.9175437958467239E-2</v>
+        <v>4.9170449720506104E-2</v>
       </c>
       <c r="L5">
-        <v>-4.4919207430038632E-4</v>
+        <v>-4.4919207430083041E-4</v>
       </c>
       <c r="M5">
-        <v>-3.0649484459494225E-2</v>
+        <v>-3.0644875722143139E-2</v>
       </c>
       <c r="N5">
-        <v>102.4265691529347</v>
+        <v>102.42656915293469</v>
       </c>
       <c r="O5">
-        <v>110.22752834938696</v>
+        <v>110.22664877495674</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1326,46 +1326,46 @@
         <v>2017</v>
       </c>
       <c r="B6">
-        <v>416.2379877064119</v>
+        <v>416.14512388109819</v>
       </c>
       <c r="C6">
         <v>8452952611.0684996</v>
       </c>
       <c r="D6">
-        <v>20307979.715274524</v>
+        <v>20312511.491745111</v>
       </c>
       <c r="E6">
-        <v>0.91906456953681659</v>
+        <v>0.9192696610944</v>
       </c>
       <c r="F6">
-        <v>125.25136685198841</v>
+        <v>125.25136685198844</v>
       </c>
       <c r="G6">
-        <v>279.95663054876223</v>
+        <v>279.89417146429003</v>
       </c>
       <c r="H6">
-        <v>-3.5969301290042055E-2</v>
+        <v>-3.5966192083694559E-2</v>
       </c>
       <c r="I6">
         <v>8.8826841671716394E-3</v>
       </c>
       <c r="J6">
-        <v>4.6525474258479083E-2</v>
+        <v>4.652209899962334E-2</v>
       </c>
       <c r="K6">
-        <v>4.2163773284719097E-2</v>
+        <v>4.2160412093241728E-2</v>
       </c>
       <c r="L6">
-        <v>1.1290411509540688E-2</v>
+        <v>1.1290411509541132E-2</v>
       </c>
       <c r="M6">
-        <v>-3.9028085741710017E-2</v>
+        <v>-3.9024986400600481E-2</v>
       </c>
       <c r="N6">
         <v>100.88826841671717</v>
       </c>
       <c r="O6">
-        <v>104.65254742584791</v>
+        <v>104.65220989996233</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1373,40 +1373,40 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>431.76839520091141</v>
+        <v>431.67067426874587</v>
       </c>
       <c r="C7">
-        <v>8378528786.0762281</v>
+        <v>8378528786.0762291</v>
       </c>
       <c r="D7">
-        <v>19405146.090365212</v>
+        <v>19409538.996990088</v>
       </c>
       <c r="E7">
-        <v>0.88188113336552165</v>
+        <v>0.88208077223734849</v>
       </c>
       <c r="F7">
-        <v>123.85301534207888</v>
+        <v>123.85301534207885</v>
       </c>
       <c r="G7">
-        <v>291.32654804468666</v>
+        <v>291.26061292262608</v>
       </c>
       <c r="H7">
-        <v>-1.9204070002918572E-2</v>
+        <v>-1.9201466363056863E-2</v>
       </c>
       <c r="I7">
         <v>6.5683161127729761E-3</v>
       </c>
       <c r="J7">
-        <v>2.6277011687607876E-2</v>
+        <v>2.6274287320018574E-2</v>
       </c>
       <c r="K7">
-        <v>1.8155459390721607E-2</v>
+        <v>1.8152756582704876E-2</v>
       </c>
       <c r="L7">
-        <v>1.6252900049103847E-2</v>
+        <v>1.6252900049103625E-2</v>
       </c>
       <c r="M7">
-        <v>-2.734775827991065E-2</v>
+        <v>-2.7345176258441239E-2</v>
       </c>
       <c r="N7">
         <v>100</v>

</xml_diff>